<commit_message>
update location arrangemnt of branches
</commit_message>
<xml_diff>
--- a/plot/dataset_based/Comparison_accuracy/comparison.xlsx
+++ b/plot/dataset_based/Comparison_accuracy/comparison.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/dataset_based/Comparison_accuracy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CA16FE-1573-EC48-BF7A-1C3FB47D93A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4941D8B2-C748-6B4F-B95C-BA257544F3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
   </bookViews>
   <sheets>
     <sheet name="accuracy" sheetId="1" r:id="rId1"/>
     <sheet name="memory" sheetId="2" r:id="rId2"/>
-    <sheet name="timeoverhead_backup" sheetId="3" r:id="rId3"/>
+    <sheet name="timeoverhead_backup" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="timeoverhead" sheetId="4" r:id="rId4"/>
+    <sheet name="timeoverhead-task=5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="46">
   <si>
     <t>MNIST</t>
   </si>
@@ -71,13 +72,7 @@
     <t>We use the ratio of YONO:Original in YONO paper to muliply the Vanilla accuracy in our own implementation to get YONO in our comparison</t>
   </si>
   <si>
-    <t>We use the ratio of NWS:Vanilla, NWV:Vanilla in NWS paper to muliply the Vanilla accuracy in our own implementation to get NWS/NWS in our comparison</t>
-  </si>
-  <si>
     <t>Accuracy</t>
-  </si>
-  <si>
-    <t>Accuracy (%) - Extracted from MWS</t>
   </si>
   <si>
     <t>Accuracy (%) - Extracted from YONO</t>
@@ -151,6 +146,36 @@
   <si>
     <t>Total Execution time of running all tasks</t>
   </si>
+  <si>
+    <t>FMNIST</t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>US8K</t>
+  </si>
+  <si>
+    <t>HHAR</t>
+  </si>
+  <si>
+    <t>Accuracy (%) - Extracted from NWS</t>
+  </si>
+  <si>
+    <t>We use the ratio of NWS:Vanilla, NWV:Vanilla in NWS paper to muliply the Vanilla accuracy in our own implementation to get NWS and NWV in our comparison</t>
+  </si>
+  <si>
+    <t>to be replaced by real data</t>
+  </si>
+  <si>
+    <t>YONO does not have the last five datasets</t>
+  </si>
+  <si>
+    <t>to be replaced with real data</t>
+  </si>
 </sst>
 </file>
 
@@ -180,7 +205,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +236,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -224,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -247,6 +284,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,28 +609,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8A6150-6557-DD49-A823-4DB21D694E8B}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A10" zoomScale="138" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -605,8 +653,23 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -630,8 +693,28 @@
         <f>F14/F16*F6</f>
         <v>70.211834639286678</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:K3" si="0">G14/G16*G6</f>
+        <v>97.511520737327189</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" si="0"/>
+        <v>99.894863202120732</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" si="0"/>
+        <v>86.387442893564256</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="0"/>
+        <v>88.378909805920685</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" si="0"/>
+        <v>89.458976713129118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -655,8 +738,28 @@
         <f>F15/F16*F6</f>
         <v>94.597676303701718</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:K4" si="1">G15/G16*G6</f>
+        <v>100.6336405529954</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>99.824738658530478</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>97.389245061801759</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>97.47205330808724</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>97.743649667529141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -680,8 +783,26 @@
         <f>F24/F25*F6</f>
         <v>93.215859030837009</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0</v>
+      </c>
+      <c r="I5" s="20">
+        <v>0</v>
+      </c>
+      <c r="J5" s="20">
+        <v>0</v>
+      </c>
+      <c r="K5" s="20">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -700,10 +821,28 @@
       <c r="F6" s="3">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="19">
+        <v>100</v>
+      </c>
+      <c r="H6" s="19">
+        <v>100</v>
+      </c>
+      <c r="I6" s="19">
+        <v>100</v>
+      </c>
+      <c r="J6" s="19">
+        <v>100</v>
+      </c>
+      <c r="K6" s="19">
+        <v>100</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>98</v>
@@ -720,18 +859,41 @@
       <c r="F7" s="3">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="19">
+        <v>100</v>
+      </c>
+      <c r="H7" s="19">
+        <v>100</v>
+      </c>
+      <c r="I7" s="19">
+        <v>100</v>
+      </c>
+      <c r="J7" s="19">
+        <v>100</v>
+      </c>
+      <c r="K7" s="19">
+        <v>100</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>0</v>
@@ -748,86 +910,146 @@
       <c r="F13" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>93.34</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>51.22</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <v>80.41</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>90.1</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <v>56.49</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="3">
+        <v>84.64</v>
+      </c>
+      <c r="H14" s="3">
+        <v>99.859899999999996</v>
+      </c>
+      <c r="I14" s="3">
+        <v>70.512799999999999</v>
+      </c>
+      <c r="J14" s="3">
+        <v>38.834400000000002</v>
+      </c>
+      <c r="K14" s="3">
+        <v>80.385599999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>98.25</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>68.900000000000006</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>87.6</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>94.34</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>76.11</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="3">
+        <v>87.35</v>
+      </c>
+      <c r="H15" s="3">
+        <v>99.7898</v>
+      </c>
+      <c r="I15" s="3">
+        <v>79.492900000000006</v>
+      </c>
+      <c r="J15" s="3">
+        <v>42.83</v>
+      </c>
+      <c r="K15" s="3">
+        <v>87.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>98.61</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>72.05</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>89.76</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>94.34</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>74.02</v>
       </c>
+      <c r="G16" s="3">
+        <v>86.8</v>
+      </c>
+      <c r="H16" s="3">
+        <v>99.965000000000003</v>
+      </c>
+      <c r="I16" s="3">
+        <v>81.623900000000006</v>
+      </c>
+      <c r="J16" s="3">
+        <v>43.940800000000003</v>
+      </c>
+      <c r="K16" s="3">
+        <v>89.857500000000002</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="A17" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="A21" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -908,22 +1130,22 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A12:F12"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -940,14 +1162,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -955,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -969,7 +1191,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4">
         <v>650</v>
@@ -1009,14 +1231,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" s="12">
         <v>5</v>
@@ -1142,7 +1364,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
@@ -1162,7 +1384,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3">
         <v>20</v>
@@ -1181,14 +1403,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="A11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1330,7 +1552,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="6">
         <f>SUM(B13:B18)</f>
@@ -1354,14 +1576,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="A22" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
@@ -1383,7 +1605,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="8">
         <f>B30/B34*D34</f>
@@ -1407,14 +1629,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="A27" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -1436,7 +1658,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B29" s="6">
         <v>65402</v>
@@ -1456,7 +1678,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B30" s="7">
         <f>B29*2/1000</f>
@@ -1483,36 +1705,36 @@
       <c r="A31" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B34" s="2">
         <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D34" s="2">
         <v>0.45700000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+      <c r="A37" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
@@ -1534,7 +1756,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B39" s="7">
         <v>14.33</v>
@@ -1554,7 +1776,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B40" s="10">
         <f>B39/B34*D34</f>
@@ -1593,10 +1815,1599 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A77F0FD-FF90-6947-BEE6-0880C6726156}">
+  <dimension ref="A1:L66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E6" sqref="E5:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7">
+        <f>B19*K1</f>
+        <v>58.61</v>
+      </c>
+      <c r="C3" s="7">
+        <f>C19*K1</f>
+        <v>97.69</v>
+      </c>
+      <c r="D3" s="7">
+        <f>D19*K1</f>
+        <v>97.69</v>
+      </c>
+      <c r="E3" s="7">
+        <f>E19*K1</f>
+        <v>98.33</v>
+      </c>
+      <c r="F3" s="7">
+        <f>F19*K1</f>
+        <v>43.470000000000006</v>
+      </c>
+      <c r="G3" s="7">
+        <f>G19*K1</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <f>H19*K1</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <f>I19*K1</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <f>J19*K1</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <f>K19*K1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7">
+        <f>B19*K1 +B66*K1</f>
+        <v>59.6332515625</v>
+      </c>
+      <c r="C4" s="7">
+        <f>C19*K1 +C66*K1</f>
+        <v>97.835668749999996</v>
+      </c>
+      <c r="D4" s="7">
+        <f>D19*K1 +D66*K1</f>
+        <v>99.444451562499992</v>
+      </c>
+      <c r="E4" s="7">
+        <f>E19*K1 +E66*K1</f>
+        <v>99.134034374999999</v>
+      </c>
+      <c r="F4" s="7">
+        <f>F19*K1+F66*K1</f>
+        <v>43.615668750000005</v>
+      </c>
+      <c r="G4" s="7">
+        <f>G19*K1+G66*K1</f>
+        <v>0.87686874999999997</v>
+      </c>
+      <c r="H4" s="7">
+        <f>H19*K1+H66*K1</f>
+        <v>0.95041718750000004</v>
+      </c>
+      <c r="I4" s="7">
+        <f>I19*K1+I66*K1</f>
+        <v>0.87686874999999997</v>
+      </c>
+      <c r="J4" s="7">
+        <f>J19*K1+J66*K1</f>
+        <v>0.21921718749999999</v>
+      </c>
+      <c r="K4" s="7">
+        <f>K19*K1+K66*K1</f>
+        <v>7.2834375000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7">
+        <f>B19*K1 + 0.024*K1</f>
+        <v>58.85</v>
+      </c>
+      <c r="C5" s="7">
+        <f>C19*K1 + 0.024*K1</f>
+        <v>97.929999999999993</v>
+      </c>
+      <c r="D5" s="7">
+        <f>D19*K1 + 0.024*K1</f>
+        <v>97.929999999999993</v>
+      </c>
+      <c r="E5" s="7">
+        <f>E19*K1 + 0.024*K1</f>
+        <v>98.57</v>
+      </c>
+      <c r="F5" s="7">
+        <f>F19*K1 + 0.024*K1</f>
+        <v>43.710000000000008</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7">
+        <f>B19*K1 + B33*K1</f>
+        <v>67.950223124999994</v>
+      </c>
+      <c r="C6" s="7">
+        <f>C19*K1 + C33*K1</f>
+        <v>106.925684375</v>
+      </c>
+      <c r="D6" s="7">
+        <f>D19*K1 + D33*K1</f>
+        <v>106.925684375</v>
+      </c>
+      <c r="E6" s="7">
+        <f>E19*K1 + E33*K1</f>
+        <v>108.19206</v>
+      </c>
+      <c r="F6" s="7">
+        <f>F19*K1 + F33*K1</f>
+        <v>52.521456250000007</v>
+      </c>
+      <c r="G6" s="7">
+        <f>G19*K1 + G33*K1</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <f>H19*K1 + H33*K1</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <f>I19*K1 + I33*K1</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <f>J19*K1 + J33*K1</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <f>K19*K1 + K33*K1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7">
+        <v>30.26</v>
+      </c>
+      <c r="C7" s="7">
+        <v>40.58</v>
+      </c>
+      <c r="D7" s="7">
+        <v>40.58</v>
+      </c>
+      <c r="E7" s="7">
+        <v>41.06</v>
+      </c>
+      <c r="F7" s="7">
+        <v>19.72</v>
+      </c>
+      <c r="G7" s="19">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0</v>
+      </c>
+      <c r="J7" s="19">
+        <v>0</v>
+      </c>
+      <c r="K7" s="19">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7">
+        <v>18.21</v>
+      </c>
+      <c r="C8" s="7">
+        <v>17.73</v>
+      </c>
+      <c r="D8" s="7">
+        <v>17.73</v>
+      </c>
+      <c r="E8" s="7">
+        <v>18.09</v>
+      </c>
+      <c r="F8" s="7">
+        <v>8.81</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="C13" s="13">
+        <v>2.57</v>
+      </c>
+      <c r="D13" s="13">
+        <v>2.57</v>
+      </c>
+      <c r="E13" s="13">
+        <v>2.6</v>
+      </c>
+      <c r="F13" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="13">
+        <v>3.81</v>
+      </c>
+      <c r="C14" s="13">
+        <v>5.25</v>
+      </c>
+      <c r="D14" s="13">
+        <v>5.25</v>
+      </c>
+      <c r="E14" s="13">
+        <v>5.28</v>
+      </c>
+      <c r="F14" s="13">
+        <v>3.01</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1.18</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1.85</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1.85</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1.86</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>4</v>
+      </c>
+      <c r="B16" s="13">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C16" s="13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D16" s="13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E16" s="13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F16" s="13">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>5</v>
+      </c>
+      <c r="B17" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="13">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D17" s="13">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E17" s="13">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F17" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>6</v>
+      </c>
+      <c r="B18" s="13">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C18" s="13">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D18" s="13">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E18" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="13">
+        <f>SUM(B13:B18)</f>
+        <v>5.8609999999999998</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" ref="C19:F19" si="0">SUM(C13:C18)</f>
+        <v>9.7690000000000001</v>
+      </c>
+      <c r="D19" s="13">
+        <f t="shared" si="0"/>
+        <v>9.7690000000000001</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>9.8330000000000002</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="0"/>
+        <v>4.3470000000000004</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>1</v>
+      </c>
+      <c r="B23" s="17">
+        <f>B50/B60*D60</f>
+        <v>2.2850000000000001E-3</v>
+      </c>
+      <c r="C23" s="17">
+        <f>C50/B60*D60</f>
+        <v>6.398E-3</v>
+      </c>
+      <c r="D23" s="17">
+        <f>D50/B60*D60</f>
+        <v>6.398E-3</v>
+      </c>
+      <c r="E23" s="17">
+        <f>E50/B60*D60</f>
+        <v>6.398E-3</v>
+      </c>
+      <c r="F23" s="17">
+        <f>F50/B60*D60</f>
+        <v>7.5405000000000003E-3</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>2</v>
+      </c>
+      <c r="B24" s="17">
+        <f>B51/B60*D60</f>
+        <v>6.6265000000000004E-2</v>
+      </c>
+      <c r="C24" s="17">
+        <f>C51/B60*D60</f>
+        <v>6.6265000000000004E-2</v>
+      </c>
+      <c r="D24" s="17">
+        <f>D51/B60*D60</f>
+        <v>6.6265000000000004E-2</v>
+      </c>
+      <c r="E24" s="17">
+        <f>E51/B60*D60</f>
+        <v>6.6265000000000004E-2</v>
+      </c>
+      <c r="F24" s="17">
+        <f>F51/B60*D60</f>
+        <v>0.23444100000000001</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>3</v>
+      </c>
+      <c r="B25" s="17">
+        <f>B52/B60*D60</f>
+        <v>0.19810949999999999</v>
+      </c>
+      <c r="C25" s="17">
+        <f>C52/B60*D60</f>
+        <v>0.21461862500000001</v>
+      </c>
+      <c r="D25" s="17">
+        <f>D52/B60*D60</f>
+        <v>0.21461862500000001</v>
+      </c>
+      <c r="E25" s="17">
+        <f>E52/B60*D60</f>
+        <v>0.21461862500000001</v>
+      </c>
+      <c r="F25" s="17">
+        <f>F52/B60*D60</f>
+        <v>0.29339400000000004</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>4</v>
+      </c>
+      <c r="B26" s="17">
+        <f>B53/B60*D60</f>
+        <v>0.17914400000000003</v>
+      </c>
+      <c r="C26" s="17">
+        <f>C53/B60*D60</f>
+        <v>0.382052</v>
+      </c>
+      <c r="D26" s="17">
+        <f>D53/B60*D60</f>
+        <v>0.382052</v>
+      </c>
+      <c r="E26" s="17">
+        <f>E53/B60*D60</f>
+        <v>0.382052</v>
+      </c>
+      <c r="F26" s="17">
+        <f>F53/B60*D60</f>
+        <v>0.23764000000000002</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17">
+        <f>B54/B60*D60</f>
+        <v>0.46979600000000005</v>
+      </c>
+      <c r="C27" s="17">
+        <f>C54/B60*D60</f>
+        <v>0.23581200000000002</v>
+      </c>
+      <c r="D27" s="17">
+        <f>D54/B60*D60</f>
+        <v>0.23581200000000002</v>
+      </c>
+      <c r="E27" s="17">
+        <f>E54/B60*D60</f>
+        <v>0.23581200000000002</v>
+      </c>
+      <c r="F27" s="17">
+        <f>F54/B60*D60</f>
+        <v>0.13213012500000001</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>6</v>
+      </c>
+      <c r="B28" s="17">
+        <f>B55/B60*D60</f>
+        <v>1.84228125E-2</v>
+      </c>
+      <c r="C28" s="17">
+        <f>C55/B60*D60</f>
+        <v>1.84228125E-2</v>
+      </c>
+      <c r="D28" s="17">
+        <f>D55/B60*D60</f>
+        <v>1.84228125E-2</v>
+      </c>
+      <c r="E28" s="17">
+        <f>E55/B60*D60</f>
+        <v>8.1060375000000004E-2</v>
+      </c>
+      <c r="F28" s="17">
+        <f>F55/B60*D60</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="17">
+        <f>SUM(B23:B28)</f>
+        <v>0.93402231250000012</v>
+      </c>
+      <c r="C29" s="17">
+        <f t="shared" ref="C29:F29" si="1">SUM(C23:C28)</f>
+        <v>0.92356843749999995</v>
+      </c>
+      <c r="D29" s="17">
+        <f t="shared" si="1"/>
+        <v>0.92356843749999995</v>
+      </c>
+      <c r="E29" s="17">
+        <f t="shared" si="1"/>
+        <v>0.98620599999999992</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="1"/>
+        <v>0.90514562500000006</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="8">
+        <f>B56/B60*D60</f>
+        <v>0.93402231250000001</v>
+      </c>
+      <c r="C33" s="8">
+        <f>C56/B60*D60</f>
+        <v>0.92356843750000006</v>
+      </c>
+      <c r="D33" s="8">
+        <f>D56/B60*D60</f>
+        <v>0.92356843750000006</v>
+      </c>
+      <c r="E33" s="8">
+        <f>E56/B60*D60</f>
+        <v>0.98620600000000003</v>
+      </c>
+      <c r="F33" s="8">
+        <f>F56/B60*D60</f>
+        <v>0.90514562500000006</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K37" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>1</v>
+      </c>
+      <c r="B38" s="13">
+        <v>160</v>
+      </c>
+      <c r="C38" s="13">
+        <v>448</v>
+      </c>
+      <c r="D38" s="13">
+        <v>448</v>
+      </c>
+      <c r="E38" s="13">
+        <v>448</v>
+      </c>
+      <c r="F38" s="13">
+        <v>528</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>2</v>
+      </c>
+      <c r="B39" s="13">
+        <v>4640</v>
+      </c>
+      <c r="C39" s="13">
+        <v>4640</v>
+      </c>
+      <c r="D39" s="13">
+        <v>4640</v>
+      </c>
+      <c r="E39" s="13">
+        <v>4640</v>
+      </c>
+      <c r="F39" s="13">
+        <v>16416</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>3</v>
+      </c>
+      <c r="B40" s="13">
+        <v>13872</v>
+      </c>
+      <c r="C40" s="13">
+        <v>15028</v>
+      </c>
+      <c r="D40" s="13">
+        <v>15028</v>
+      </c>
+      <c r="E40" s="13">
+        <v>15028</v>
+      </c>
+      <c r="F40" s="13">
+        <v>20544</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>4</v>
+      </c>
+      <c r="B41" s="13">
+        <v>12544</v>
+      </c>
+      <c r="C41" s="13">
+        <v>26752</v>
+      </c>
+      <c r="D41" s="13">
+        <v>26752</v>
+      </c>
+      <c r="E41" s="13">
+        <v>26752</v>
+      </c>
+      <c r="F41" s="13">
+        <v>16640</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>5</v>
+      </c>
+      <c r="B42" s="13">
+        <v>32896</v>
+      </c>
+      <c r="C42" s="13">
+        <v>16512</v>
+      </c>
+      <c r="D42" s="13">
+        <v>16512</v>
+      </c>
+      <c r="E42" s="13">
+        <v>16512</v>
+      </c>
+      <c r="F42" s="13">
+        <v>9252</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>6</v>
+      </c>
+      <c r="B43" s="13">
+        <v>1290</v>
+      </c>
+      <c r="C43" s="13">
+        <v>1290</v>
+      </c>
+      <c r="D43" s="13">
+        <v>1290</v>
+      </c>
+      <c r="E43" s="13">
+        <v>5676</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="13">
+        <f>SUM(B38:B43)</f>
+        <v>65402</v>
+      </c>
+      <c r="C44" s="13">
+        <f t="shared" ref="C44:F44" si="2">SUM(C38:C43)</f>
+        <v>64670</v>
+      </c>
+      <c r="D44" s="13">
+        <f t="shared" si="2"/>
+        <v>64670</v>
+      </c>
+      <c r="E44" s="13">
+        <f t="shared" si="2"/>
+        <v>69056</v>
+      </c>
+      <c r="F44" s="13">
+        <f t="shared" si="2"/>
+        <v>63380</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="14">
+        <f>B44*2/1000</f>
+        <v>130.804</v>
+      </c>
+      <c r="C45" s="14">
+        <f t="shared" ref="C45:F45" si="3">C44*2/1000</f>
+        <v>129.34</v>
+      </c>
+      <c r="D45" s="14">
+        <f t="shared" si="3"/>
+        <v>129.34</v>
+      </c>
+      <c r="E45" s="14">
+        <f t="shared" si="3"/>
+        <v>138.11199999999999</v>
+      </c>
+      <c r="F45" s="14">
+        <f t="shared" si="3"/>
+        <v>126.76</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="9"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I49" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J49" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K49" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>1</v>
+      </c>
+      <c r="B50" s="13">
+        <f>B38*2/1000</f>
+        <v>0.32</v>
+      </c>
+      <c r="C50" s="13">
+        <f t="shared" ref="C50:F50" si="4">C38*2/1000</f>
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="D50" s="13">
+        <f t="shared" si="4"/>
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="E50" s="13">
+        <f t="shared" si="4"/>
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="F50" s="13">
+        <f t="shared" si="4"/>
+        <v>1.056</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>2</v>
+      </c>
+      <c r="B51" s="13">
+        <f t="shared" ref="B51:F55" si="5">B39*2/1000</f>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="C51" s="13">
+        <f t="shared" si="5"/>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="D51" s="13">
+        <f t="shared" si="5"/>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="E51" s="13">
+        <f t="shared" si="5"/>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="F51" s="13">
+        <f t="shared" si="5"/>
+        <v>32.832000000000001</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>3</v>
+      </c>
+      <c r="B52" s="13">
+        <f t="shared" si="5"/>
+        <v>27.744</v>
+      </c>
+      <c r="C52" s="13">
+        <f t="shared" si="5"/>
+        <v>30.056000000000001</v>
+      </c>
+      <c r="D52" s="13">
+        <f t="shared" si="5"/>
+        <v>30.056000000000001</v>
+      </c>
+      <c r="E52" s="13">
+        <f t="shared" si="5"/>
+        <v>30.056000000000001</v>
+      </c>
+      <c r="F52" s="13">
+        <f t="shared" si="5"/>
+        <v>41.088000000000001</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>4</v>
+      </c>
+      <c r="B53" s="13">
+        <f t="shared" si="5"/>
+        <v>25.088000000000001</v>
+      </c>
+      <c r="C53" s="13">
+        <f t="shared" si="5"/>
+        <v>53.503999999999998</v>
+      </c>
+      <c r="D53" s="13">
+        <f t="shared" si="5"/>
+        <v>53.503999999999998</v>
+      </c>
+      <c r="E53" s="13">
+        <f t="shared" si="5"/>
+        <v>53.503999999999998</v>
+      </c>
+      <c r="F53" s="13">
+        <f t="shared" si="5"/>
+        <v>33.28</v>
+      </c>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>5</v>
+      </c>
+      <c r="B54" s="13">
+        <f t="shared" si="5"/>
+        <v>65.792000000000002</v>
+      </c>
+      <c r="C54" s="13">
+        <f t="shared" si="5"/>
+        <v>33.024000000000001</v>
+      </c>
+      <c r="D54" s="13">
+        <f t="shared" si="5"/>
+        <v>33.024000000000001</v>
+      </c>
+      <c r="E54" s="13">
+        <f t="shared" si="5"/>
+        <v>33.024000000000001</v>
+      </c>
+      <c r="F54" s="13">
+        <f t="shared" si="5"/>
+        <v>18.504000000000001</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>6</v>
+      </c>
+      <c r="B55" s="13">
+        <f t="shared" si="5"/>
+        <v>2.58</v>
+      </c>
+      <c r="C55" s="13">
+        <f t="shared" si="5"/>
+        <v>2.58</v>
+      </c>
+      <c r="D55" s="13">
+        <f t="shared" si="5"/>
+        <v>2.58</v>
+      </c>
+      <c r="E55" s="13">
+        <f t="shared" si="5"/>
+        <v>11.352</v>
+      </c>
+      <c r="F55" s="13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="13">
+        <f>SUM(B50:B55)</f>
+        <v>130.804</v>
+      </c>
+      <c r="C56" s="13">
+        <f t="shared" ref="C56" si="6">SUM(C50:C55)</f>
+        <v>129.34</v>
+      </c>
+      <c r="D56" s="13">
+        <f t="shared" ref="D56" si="7">SUM(D50:D55)</f>
+        <v>129.34</v>
+      </c>
+      <c r="E56" s="13">
+        <f t="shared" ref="E56" si="8">SUM(E50:E55)</f>
+        <v>138.11199999999999</v>
+      </c>
+      <c r="F56" s="13">
+        <f t="shared" ref="F56" si="9">SUM(F50:F55)</f>
+        <v>126.76</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="2">
+        <v>64</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.45700000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I64" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J64" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K64" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="7">
+        <v>14.33</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2.04</v>
+      </c>
+      <c r="D65" s="7">
+        <v>24.57</v>
+      </c>
+      <c r="E65" s="7">
+        <v>11.26</v>
+      </c>
+      <c r="F65" s="7">
+        <v>2.04</v>
+      </c>
+      <c r="G65" s="3">
+        <v>12.28</v>
+      </c>
+      <c r="H65" s="3">
+        <v>13.31</v>
+      </c>
+      <c r="I65" s="3">
+        <v>12.28</v>
+      </c>
+      <c r="J65" s="3">
+        <v>3.07</v>
+      </c>
+      <c r="K65" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="10">
+        <f>B65/B60*D60</f>
+        <v>0.10232515625000001</v>
+      </c>
+      <c r="C66" s="10">
+        <f>C65/B60*D60</f>
+        <v>1.4566875E-2</v>
+      </c>
+      <c r="D66" s="10">
+        <f>D65/B60*D60</f>
+        <v>0.17544515625000001</v>
+      </c>
+      <c r="E66" s="10">
+        <f>E65/B60*D60</f>
+        <v>8.0403437500000008E-2</v>
+      </c>
+      <c r="F66" s="10">
+        <f>F65/B60*D60</f>
+        <v>1.4566875E-2</v>
+      </c>
+      <c r="G66" s="10">
+        <f>G65/B60*D60</f>
+        <v>8.7686874999999997E-2</v>
+      </c>
+      <c r="H66" s="3">
+        <f>H65/B60*D60</f>
+        <v>9.5041718750000004E-2</v>
+      </c>
+      <c r="I66" s="3">
+        <f>I65/B60*D60</f>
+        <v>8.7686874999999997E-2</v>
+      </c>
+      <c r="J66" s="3">
+        <f>J65/B60*D60</f>
+        <v>2.1921718749999999E-2</v>
+      </c>
+      <c r="K66" s="3">
+        <f>K65/B60*D60</f>
+        <v>7.2834375E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A63:K63"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A31:K31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G3:G4 G6" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BB6D28-0DA4-6B47-9767-B86832CEED60}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1605,14 +3416,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" s="12">
         <v>5</v>
@@ -1738,7 +3549,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="7">
         <v>30.26</v>
@@ -1758,7 +3569,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7">
         <v>18.21</v>
@@ -1777,18 +3588,18 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="A11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -1928,7 +3739,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="13">
         <f>SUM(B13:B18)</f>
@@ -1952,18 +3763,18 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="A21" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
@@ -2133,7 +3944,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" s="17">
         <f>SUM(B23:B28)</f>
@@ -2157,14 +3968,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="A31" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -2186,7 +3997,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B33" s="8">
         <f>B56/B60*D60</f>
@@ -2210,18 +4021,18 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+      <c r="A36" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>0</v>
@@ -2361,7 +4172,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B44" s="13">
         <f>SUM(B38:B43)</f>
@@ -2386,7 +4197,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B45" s="14">
         <f>B44*2/1000</f>
@@ -2420,18 +4231,18 @@
       <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="A48" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>0</v>
@@ -2601,26 +4412,26 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B56" s="13">
         <f>SUM(B50:B55)</f>
         <v>130.804</v>
       </c>
       <c r="C56" s="13">
-        <f t="shared" ref="C56" si="6">SUM(C50:C55)</f>
+        <f t="shared" ref="C56:F56" si="6">SUM(C50:C55)</f>
         <v>129.34</v>
       </c>
       <c r="D56" s="13">
-        <f t="shared" ref="D56" si="7">SUM(D50:D55)</f>
+        <f t="shared" si="6"/>
         <v>129.34</v>
       </c>
       <c r="E56" s="13">
-        <f t="shared" ref="E56" si="8">SUM(E50:E55)</f>
+        <f t="shared" si="6"/>
         <v>138.11199999999999</v>
       </c>
       <c r="F56" s="13">
-        <f t="shared" ref="F56" si="9">SUM(F50:F55)</f>
+        <f t="shared" si="6"/>
         <v>126.76</v>
       </c>
     </row>
@@ -2632,36 +4443,36 @@
       <c r="F57" s="15"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
+      <c r="A59" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B60" s="2">
         <v>64</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D60" s="2">
         <v>0.45700000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
+      <c r="A63" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -2683,7 +4494,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B65" s="7">
         <v>14.33</v>
@@ -2703,7 +4514,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B66" s="10">
         <f>B65/B60*D60</f>
@@ -2728,14 +4539,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A59:D59"/>
     <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A48:F48"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A21:F21"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A48:F48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update font of some figures
</commit_message>
<xml_diff>
--- a/plot/dataset_based/Comparison_accuracy/comparison.xlsx
+++ b/plot/dataset_based/Comparison_accuracy/comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/dataset_based/Comparison_accuracy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA29D75-9367-9D44-AD65-B17F8193C290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF050B8-8227-3440-9A92-480896605BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="55">
   <si>
     <t>MNIST</t>
   </si>
@@ -203,6 +203,9 @@
   <si>
     <t>Total energy overhead of running all tasks (mJ)</t>
   </si>
+  <si>
+    <t>CIFAR</t>
+  </si>
 </sst>
 </file>
 
@@ -319,13 +322,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,7 +646,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,18 +656,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -672,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -854,31 +857,31 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="23">
         <v>99.6</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="23">
         <v>94.6</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>98.4</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>100</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <v>98.4</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <v>99.7</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="23">
         <v>99.4</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <v>97.1</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="23">
         <v>96.4</v>
       </c>
     </row>
@@ -915,18 +918,18 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -1055,24 +1058,24 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
@@ -1153,14 +1156,14 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1185,14 +1188,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1254,12 +1257,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="12" t="s">
         <v>27</v>
       </c>
@@ -1426,14 +1429,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1599,14 +1602,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
@@ -1652,14 +1655,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -1728,12 +1731,12 @@
       <c r="A31" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -1750,14 +1753,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
@@ -1850,16 +1853,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="12" t="s">
         <v>27</v>
       </c>
@@ -2175,18 +2178,18 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -2454,18 +2457,18 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -2787,18 +2790,18 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -2872,18 +2875,18 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -3202,18 +3205,18 @@
       <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -3542,12 +3545,12 @@
       <c r="F57" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -3564,18 +3567,18 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -3712,16 +3715,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="12" t="s">
         <v>27</v>
       </c>
@@ -4036,18 +4039,18 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -4315,18 +4318,18 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -4648,18 +4651,18 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -4733,18 +4736,18 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -5063,18 +5066,18 @@
       <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -5403,12 +5406,12 @@
       <c r="F57" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -5425,18 +5428,18 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -5570,16 +5573,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="12" t="s">
         <v>27</v>
       </c>
@@ -5895,18 +5898,18 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -6174,18 +6177,18 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -6507,18 +6510,18 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -6592,18 +6595,18 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -6922,18 +6925,18 @@
       <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -7262,12 +7265,12 @@
       <c r="F57" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -7284,18 +7287,18 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -7429,16 +7432,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="12" t="s">
         <v>27</v>
       </c>
@@ -7754,18 +7757,18 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -8033,18 +8036,18 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -8366,18 +8369,18 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -8451,18 +8454,18 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -8781,18 +8784,18 @@
       <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -9121,12 +9124,12 @@
       <c r="F57" s="15"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -9143,18 +9146,18 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="23"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -9288,12 +9291,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="12" t="s">
         <v>27</v>
       </c>
@@ -9460,14 +9463,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -9635,14 +9638,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -9840,14 +9843,14 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -9893,14 +9896,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -10103,14 +10106,14 @@
       <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -10315,12 +10318,12 @@
       <c r="F57" s="15"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -10337,14 +10340,14 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>

</xml_diff>